<commit_message>
Presupuesto Conceptos para revision
</commit_message>
<xml_diff>
--- a/Practica_4/Libro1.xlsx
+++ b/Practica_4/Libro1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto por conceptos" sheetId="1" r:id="rId1"/>
@@ -168,9 +168,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -267,7 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda [0]" xfId="1" builtinId="7"/>
@@ -552,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +577,7 @@
       </c>
       <c r="B3" s="13">
         <f>SUM(B4:B5)</f>
-        <v>1598247.1574999997</v>
+        <v>1602542.6549999998</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,7 +586,7 @@
       </c>
       <c r="B4" s="15">
         <f>306609.85*3.5-B23</f>
-        <v>1065498.1049999997</v>
+        <v>1068361.7699999998</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -594,7 +595,7 @@
       </c>
       <c r="B5" s="16">
         <f>B4/2</f>
-        <v>532749.05249999987</v>
+        <v>534180.88499999989</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -603,7 +604,7 @@
       </c>
       <c r="B6" s="15">
         <f>B7+B14+B22</f>
-        <v>40091.221666666665</v>
+        <v>35795.724166666667</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -738,7 +739,7 @@
       </c>
       <c r="B22" s="8">
         <f>SUM(B23:B24)</f>
-        <v>11454.555</v>
+        <v>7159.0574999999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -746,8 +747,8 @@
         <v>21</v>
       </c>
       <c r="B23" s="5">
-        <f>2181.82*3.5</f>
-        <v>7636.3700000000008</v>
+        <f>1363.63*3.5</f>
+        <v>4772.7049999999999</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -756,7 +757,7 @@
       </c>
       <c r="B24" s="5">
         <f>B23/2</f>
-        <v>3818.1850000000004</v>
+        <v>2386.3525</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -926,7 +927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1383,7 +1386,7 @@
       </c>
       <c r="B6" s="8">
         <f t="shared" ref="B6:Z6" si="2">B7+B12+B13</f>
-        <v>-32316.221666666665</v>
+        <v>-20861.666666666664</v>
       </c>
       <c r="C6" s="8">
         <f t="shared" si="2"/>
@@ -1411,7 +1414,7 @@
       </c>
       <c r="I6" s="8">
         <f t="shared" si="2"/>
-        <v>-4028.1850000000004</v>
+        <v>-2596.3700000000003</v>
       </c>
       <c r="J6" s="8">
         <f t="shared" si="2"/>
@@ -1439,7 +1442,7 @@
       </c>
       <c r="P6" s="8">
         <f t="shared" si="2"/>
-        <v>-4028.1850000000004</v>
+        <v>-2596.3700000000003</v>
       </c>
       <c r="Q6" s="8">
         <f t="shared" si="2"/>
@@ -1475,7 +1478,7 @@
       </c>
       <c r="Y6" s="8">
         <f t="shared" si="2"/>
-        <v>-4028.1850000000004</v>
+        <v>-2596.3700000000003</v>
       </c>
       <c r="Z6" s="8">
         <f t="shared" si="2"/>
@@ -2067,7 +2070,7 @@
       </c>
       <c r="B13" s="8">
         <f>SUM(B14:B15)</f>
-        <v>-11454.555</v>
+        <v>0</v>
       </c>
       <c r="C13" s="8">
         <f t="shared" ref="C13:Z13" si="4">SUM(C14:C15)</f>
@@ -2095,7 +2098,7 @@
       </c>
       <c r="I13" s="8">
         <f t="shared" si="4"/>
-        <v>-3818.1850000000004</v>
+        <v>-2386.3700000000003</v>
       </c>
       <c r="J13" s="8">
         <f t="shared" si="4"/>
@@ -2123,7 +2126,7 @@
       </c>
       <c r="P13" s="8">
         <f t="shared" si="4"/>
-        <v>-3818.1850000000004</v>
+        <v>-2386.3700000000003</v>
       </c>
       <c r="Q13" s="8">
         <f t="shared" si="4"/>
@@ -2159,7 +2162,7 @@
       </c>
       <c r="Y13" s="8">
         <f t="shared" si="4"/>
-        <v>-3818.1850000000004</v>
+        <v>-2386.3700000000003</v>
       </c>
       <c r="Z13" s="8">
         <f t="shared" si="4"/>
@@ -2181,8 +2184,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="5">
-        <f>-2181.82*3.5</f>
-        <v>-7636.3700000000008</v>
+        <v>0</v>
       </c>
       <c r="C14" s="5">
         <v>0</v>
@@ -2203,8 +2205,8 @@
         <v>0</v>
       </c>
       <c r="I14" s="5">
-        <f>-2181.82*3.5/3</f>
-        <v>-2545.4566666666669</v>
+        <f>-1363.64*3.5/3</f>
+        <v>-1590.9133333333336</v>
       </c>
       <c r="J14" s="5">
         <v>0</v>
@@ -2225,8 +2227,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="5">
-        <f>-2181.82*3.5/3</f>
-        <v>-2545.4566666666669</v>
+        <v>-1590.9133333333336</v>
       </c>
       <c r="Q14" s="5">
         <v>0</v>
@@ -2253,8 +2254,7 @@
         <v>0</v>
       </c>
       <c r="Y14" s="5">
-        <f>-2181.82*3.5/3</f>
-        <v>-2545.4566666666669</v>
+        <v>-1590.9133333333336</v>
       </c>
       <c r="Z14" s="5">
         <v>0</v>
@@ -2275,8 +2275,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="5">
-        <f>B14/2</f>
-        <v>-3818.1850000000004</v>
+        <v>0</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" ref="C15:Z15" si="5">C14/2</f>
@@ -2304,7 +2303,7 @@
       </c>
       <c r="I15" s="5">
         <f>I14/2</f>
-        <v>-1272.7283333333335</v>
+        <v>-795.45666666666682</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="5"/>
@@ -2332,7 +2331,7 @@
       </c>
       <c r="P15" s="5">
         <f>P14/2</f>
-        <v>-1272.7283333333335</v>
+        <v>-795.45666666666682</v>
       </c>
       <c r="Q15" s="5">
         <f t="shared" si="5"/>
@@ -2368,7 +2367,7 @@
       </c>
       <c r="Y15" s="5">
         <f>Y14/2</f>
-        <v>-1272.7283333333335</v>
+        <v>-795.45666666666682</v>
       </c>
       <c r="Z15" s="5">
         <f t="shared" si="5"/>
@@ -3035,7 +3034,7 @@
         <v>-83.333333333333329</v>
       </c>
       <c r="C22" s="8">
-        <f t="shared" ref="C22:Z22" si="10">-2000/24</f>
+        <f t="shared" ref="C22:Y22" si="10">-2000/24</f>
         <v>-83.333333333333329</v>
       </c>
       <c r="D22" s="8">
@@ -3146,10 +3145,10 @@
       </c>
       <c r="B23" s="8">
         <f>B3+B6+B16</f>
-        <v>-99375.766666666663</v>
+        <v>-87921.21166666667</v>
       </c>
       <c r="C23" s="8">
-        <f t="shared" ref="C23:Z23" si="11">C3+C6+C16</f>
+        <f t="shared" ref="C23:Y23" si="11">C3+C6+C16</f>
         <v>-67268.044999999998</v>
       </c>
       <c r="D23" s="8">
@@ -3174,7 +3173,7 @@
       </c>
       <c r="I23" s="8">
         <f t="shared" si="11"/>
-        <v>-71243.896666666667</v>
+        <v>-69812.081666666665</v>
       </c>
       <c r="J23" s="8">
         <f t="shared" si="11"/>
@@ -3202,7 +3201,7 @@
       </c>
       <c r="P23" s="8">
         <f t="shared" si="11"/>
-        <v>-71233.396666666667</v>
+        <v>-69801.581666666665</v>
       </c>
       <c r="Q23" s="8">
         <f t="shared" si="11"/>
@@ -3238,7 +3237,7 @@
       </c>
       <c r="Y23" s="8">
         <f t="shared" si="11"/>
-        <v>-71719.896666666667</v>
+        <v>-70288.081666666665</v>
       </c>
       <c r="Z23" s="8">
         <f>Z2</f>
@@ -3265,8 +3264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3286,7 +3285,7 @@
       </c>
       <c r="B1" s="8">
         <f>'Flujo de Caja'!B23</f>
-        <v>-99375.766666666663</v>
+        <v>-87921.21166666667</v>
       </c>
       <c r="C1" s="8">
         <f>'Flujo de Caja'!C23</f>
@@ -3314,7 +3313,7 @@
       </c>
       <c r="I1" s="8">
         <f>'Flujo de Caja'!I23</f>
-        <v>-71243.896666666667</v>
+        <v>-69812.081666666665</v>
       </c>
       <c r="J1" s="8">
         <f>'Flujo de Caja'!J23</f>
@@ -3342,7 +3341,7 @@
       </c>
       <c r="P1" s="8">
         <f>'Flujo de Caja'!P23</f>
-        <v>-71233.396666666667</v>
+        <v>-69801.581666666665</v>
       </c>
       <c r="Q1" s="8">
         <f>'Flujo de Caja'!Q23</f>
@@ -3378,7 +3377,7 @@
       </c>
       <c r="Y1" s="8">
         <f>'Flujo de Caja'!Y23</f>
-        <v>-71719.896666666667</v>
+        <v>-70288.081666666665</v>
       </c>
       <c r="Z1" s="8">
         <f>'Flujo de Caja'!Z23</f>
@@ -3468,103 +3467,103 @@
       </c>
       <c r="B3" s="5">
         <f>B1</f>
-        <v>-99375.766666666663</v>
+        <v>-87921.21166666667</v>
       </c>
       <c r="C3" s="5">
         <f>B3+C1</f>
-        <v>-166643.81166666665</v>
+        <v>-155189.25666666665</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" ref="D3:Z3" si="0">C3+D1</f>
-        <v>-233910.35666666663</v>
+        <v>-222455.80166666664</v>
       </c>
       <c r="E3" s="5">
         <f t="shared" si="0"/>
-        <v>-301175.40166666661</v>
+        <v>-289720.84666666662</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" si="0"/>
-        <v>-368438.9466666666</v>
+        <v>-356984.3916666666</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="0"/>
-        <v>-435700.99166666658</v>
+        <v>-424246.43666666659</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="0"/>
-        <v>-502961.53666666656</v>
+        <v>-491506.98166666657</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" si="0"/>
-        <v>-574205.43333333323</v>
+        <v>-561319.06333333324</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" si="0"/>
-        <v>-641462.97833333327</v>
+        <v>-628576.60833333328</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" si="0"/>
-        <v>-708719.02333333332</v>
+        <v>-695832.65333333332</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" si="0"/>
-        <v>-775973.56833333336</v>
+        <v>-763087.19833333336</v>
       </c>
       <c r="M3" s="5">
         <f t="shared" si="0"/>
-        <v>-846671.6133333334</v>
+        <v>-833785.2433333334</v>
       </c>
       <c r="N3" s="5">
         <f t="shared" si="0"/>
-        <v>586076.84166666667</v>
+        <v>598963.21166666667</v>
       </c>
       <c r="O3" s="5">
         <f t="shared" si="0"/>
-        <v>518826.79666666669</v>
+        <v>531713.16666666663</v>
       </c>
       <c r="P3" s="5">
         <f t="shared" si="0"/>
-        <v>447593.4</v>
+        <v>461911.58499999996</v>
       </c>
       <c r="Q3" s="5">
         <f t="shared" si="0"/>
-        <v>380346.35500000004</v>
+        <v>394664.54</v>
       </c>
       <c r="R3" s="5">
         <f t="shared" si="0"/>
-        <v>313100.81000000006</v>
+        <v>327418.995</v>
       </c>
       <c r="S3" s="5">
         <f t="shared" si="0"/>
-        <v>245856.76500000007</v>
+        <v>260174.95</v>
       </c>
       <c r="T3" s="5">
         <f t="shared" si="0"/>
-        <v>178614.22000000009</v>
+        <v>192932.40500000003</v>
       </c>
       <c r="U3" s="5">
         <f t="shared" si="0"/>
-        <v>111373.17500000009</v>
+        <v>125691.36000000003</v>
       </c>
       <c r="V3" s="5">
         <f t="shared" si="0"/>
-        <v>44133.630000000092</v>
+        <v>58451.815000000031</v>
       </c>
       <c r="W3" s="5">
         <f t="shared" si="0"/>
-        <v>-23104.414999999906</v>
+        <v>-8786.2299999999668</v>
       </c>
       <c r="X3" s="5">
         <f t="shared" si="0"/>
-        <v>-90340.959999999905</v>
+        <v>-76022.774999999965</v>
       </c>
       <c r="Y3" s="5">
         <f t="shared" si="0"/>
-        <v>-162060.85666666657</v>
+        <v>-146310.85666666663</v>
       </c>
       <c r="Z3" s="5">
         <f t="shared" si="0"/>
-        <v>1337939.1433333335</v>
+        <v>1353689.1433333333</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -3581,39 +3580,39 @@
       </c>
       <c r="B7" s="5">
         <f>B3</f>
-        <v>-99375.766666666663</v>
+        <v>-87921.21166666667</v>
       </c>
       <c r="E7" s="5">
         <f>E3/(1+B5)</f>
-        <v>-278479.33579904452</v>
+        <v>-267887.97657574352</v>
       </c>
       <c r="H7" s="5">
         <f>H3/(1+B5)^2</f>
-        <v>-430013.14005771134</v>
+        <v>-420219.92764596752</v>
       </c>
       <c r="K7" s="5">
         <f>K3/(1+B5)^3</f>
-        <v>-560266.32374768809</v>
+        <v>-550079.21304703911</v>
       </c>
       <c r="N7" s="5">
         <f>N3/(1+B5)^4</f>
-        <v>428399.01720305212</v>
+        <v>437818.44457304658</v>
       </c>
       <c r="Q7" s="5">
         <f>Q3/(1+B5)^5</f>
-        <v>257067.18374026328</v>
+        <v>266744.50927746232</v>
       </c>
       <c r="T7" s="5">
         <f>T3/(1+B5)^6</f>
-        <v>111623.8220132303</v>
+        <v>120571.8807623741</v>
       </c>
       <c r="W7" s="5">
         <f>W3/(1+B5)^7</f>
-        <v>-13350.862105201244</v>
+        <v>-5077.1138396961087</v>
       </c>
       <c r="Z7" s="5">
         <f>Z3/(1+B5)^8</f>
-        <v>714865.2225942876</v>
+        <v>723280.49866417598</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -3651,7 +3650,7 @@
       </c>
       <c r="B10" s="8">
         <f>SUM(B7:Z7)</f>
-        <v>130469.81717452162</v>
+        <v>217229.89050194598</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -3659,7 +3658,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="20">
-        <v>0.1057</v>
+        <v>0.12255000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Presupuesto por tareas, VAN y TIR hechos
</commit_message>
<xml_diff>
--- a/Practica_4/Libro1.xlsx
+++ b/Practica_4/Libro1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto por conceptos" sheetId="1" r:id="rId1"/>
@@ -233,7 +233,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -269,6 +269,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda [0]" xfId="1" builtinId="7"/>
@@ -553,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +839,7 @@
   <dimension ref="A2:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,8 +906,8 @@
         <v>37</v>
       </c>
       <c r="B8" s="11">
-        <f>'Presupuesto por conceptos'!B32*0.0126</f>
-        <v>20699.763577499998</v>
+        <f>'Presupuesto por conceptos'!B32*0.014</f>
+        <v>22999.73730833333</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -915,7 +916,7 @@
       </c>
       <c r="B9" s="5">
         <f>SUM(B3:B8)</f>
-        <v>1640538.4054358331</v>
+        <v>1642838.3791666667</v>
       </c>
     </row>
   </sheetData>
@@ -927,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,6 +940,7 @@
     <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -1022,7 +1024,9 @@
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5">
+        <v>-100000</v>
+      </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1049,9 +1053,12 @@
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5">
-        <v>1500000</v>
-      </c>
-      <c r="AA2" s="5"/>
+        <f>1500000+AA2</f>
+        <v>1687159.6400000001</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>187159.64</v>
+      </c>
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
@@ -1072,95 +1079,95 @@
       </c>
       <c r="C3" s="8">
         <f t="shared" ref="C3:Y3" si="0">SUM(C4:C5)</f>
-        <v>-66933.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="D3" s="8">
         <f t="shared" si="0"/>
-        <v>-66931.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="E3" s="8">
         <f t="shared" si="0"/>
-        <v>-66930.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="F3" s="8">
         <f t="shared" si="0"/>
-        <v>-66928.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="G3" s="8">
         <f t="shared" si="0"/>
-        <v>-66927.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="H3" s="8">
         <f t="shared" si="0"/>
-        <v>-66925.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="I3" s="8">
         <f t="shared" si="0"/>
-        <v>-66924.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="J3" s="8">
         <f t="shared" si="0"/>
-        <v>-66922.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="K3" s="8">
         <f t="shared" si="0"/>
-        <v>-66921.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="L3" s="8">
         <f t="shared" si="0"/>
-        <v>-66919.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="M3" s="8">
         <f t="shared" si="0"/>
-        <v>-66918.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="N3" s="8">
         <f t="shared" si="0"/>
-        <v>-66916.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="O3" s="8">
         <f t="shared" si="0"/>
-        <v>-66915.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="P3" s="8">
         <f t="shared" si="0"/>
-        <v>-66913.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="Q3" s="8">
         <f t="shared" si="0"/>
-        <v>-66912.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="R3" s="8">
         <f t="shared" si="0"/>
-        <v>-66910.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="S3" s="8">
         <f t="shared" si="0"/>
-        <v>-66909.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="T3" s="8">
         <f t="shared" si="0"/>
-        <v>-66907.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="U3" s="8">
         <f t="shared" si="0"/>
-        <v>-66906.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="V3" s="8">
         <f t="shared" si="0"/>
-        <v>-66904.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="W3" s="8">
         <f t="shared" si="0"/>
-        <v>-66903.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="X3" s="8">
         <f t="shared" si="0"/>
-        <v>-66901.544999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="Y3" s="8">
         <f t="shared" si="0"/>
-        <v>-66900.044999999998</v>
+        <v>-66934.544999999998</v>
       </c>
       <c r="Z3" s="8">
         <v>0</v>
@@ -1184,73 +1191,96 @@
         <v>-44623.03</v>
       </c>
       <c r="C4" s="5">
-        <v>-44622.03</v>
+        <f>B4</f>
+        <v>-44623.03</v>
       </c>
       <c r="D4" s="5">
-        <v>-44621.03</v>
+        <f t="shared" ref="D4:Y4" si="1">C4</f>
+        <v>-44623.03</v>
       </c>
       <c r="E4" s="5">
-        <v>-44620.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="F4" s="5">
-        <v>-44619.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="G4" s="5">
-        <v>-44618.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="H4" s="5">
-        <v>-44617.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="I4" s="5">
-        <v>-44616.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="J4" s="5">
-        <v>-44615.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="K4" s="5">
-        <v>-44614.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="L4" s="5">
-        <v>-44613.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="M4" s="5">
-        <v>-44612.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="N4" s="5">
-        <v>-44611.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="O4" s="5">
-        <v>-44610.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="P4" s="5">
-        <v>-44609.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="Q4" s="5">
-        <v>-44608.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="R4" s="5">
-        <v>-44607.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="S4" s="5">
-        <v>-44606.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="T4" s="5">
-        <v>-44605.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="U4" s="5">
-        <v>-44604.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="V4" s="5">
-        <v>-44603.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="W4" s="5">
-        <v>-44602.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="X4" s="5">
-        <v>-44601.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="Y4" s="5">
-        <v>-44600.03</v>
+        <f t="shared" si="1"/>
+        <v>-44623.03</v>
       </c>
       <c r="Z4" s="5">
         <v>0</v>
@@ -1275,96 +1305,96 @@
         <v>-22311.514999999999</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:Y5" si="1">C4/2</f>
-        <v>-22311.014999999999</v>
+        <f t="shared" ref="C5:Y5" si="2">C4/2</f>
+        <v>-22311.514999999999</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22310.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22310.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22309.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22309.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22308.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22308.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22307.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22307.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22306.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22306.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22305.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="O5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22305.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="P5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22304.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22304.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="R5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22303.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="S5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22303.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="T5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22302.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="U5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22302.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="V5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22301.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="W5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22301.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="X5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22300.514999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="Y5" s="4">
-        <f t="shared" si="1"/>
-        <v>-22300.014999999999</v>
+        <f t="shared" si="2"/>
+        <v>-22311.514999999999</v>
       </c>
       <c r="Z5" s="4">
         <v>0</v>
@@ -1385,103 +1415,103 @@
         <v>4</v>
       </c>
       <c r="B6" s="8">
-        <f t="shared" ref="B6:Z6" si="2">B7+B12+B13</f>
+        <f t="shared" ref="B6:Z6" si="3">B7+B12+B13</f>
         <v>-20861.666666666664</v>
       </c>
       <c r="C6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="E6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="G6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="H6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="I6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2596.3700000000003</v>
       </c>
       <c r="J6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="K6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="L6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="M6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3155</v>
       </c>
       <c r="N6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="O6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="P6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2596.3700000000003</v>
       </c>
       <c r="Q6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="R6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="S6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="T6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="U6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="V6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="W6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="X6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
       <c r="Y6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-2596.3700000000003</v>
       </c>
       <c r="Z6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA6" s="5"/>
@@ -1504,99 +1534,99 @@
         <v>-20387.666666666664</v>
       </c>
       <c r="C7" s="8">
-        <f t="shared" ref="C7:Z7" si="3">SUM(C8:C11)</f>
+        <f t="shared" ref="C7:Z7" si="4">SUM(C8:C11)</f>
         <v>-210</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="E7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="G7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="I7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="J7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="K7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="L7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="M7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3155</v>
       </c>
       <c r="N7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="O7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="P7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="Q7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="R7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="S7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="T7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="U7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="V7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="W7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="X7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="Y7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-210</v>
       </c>
       <c r="Z7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AA7" s="5"/>
@@ -2073,99 +2103,99 @@
         <v>0</v>
       </c>
       <c r="C13" s="8">
-        <f t="shared" ref="C13:Z13" si="4">SUM(C14:C15)</f>
+        <f t="shared" ref="C13:Z13" si="5">SUM(C14:C15)</f>
         <v>0</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2386.3700000000003</v>
       </c>
       <c r="J13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2386.3700000000003</v>
       </c>
       <c r="Q13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2386.3700000000003</v>
       </c>
       <c r="Z13" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA13" s="5"/>
@@ -2278,27 +2308,27 @@
         <v>0</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" ref="C15:Z15" si="5">C14/2</f>
+        <f t="shared" ref="C15:Z15" si="6">C14/2</f>
         <v>0</v>
       </c>
       <c r="D15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I15" s="5">
@@ -2306,27 +2336,27 @@
         <v>-795.45666666666682</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P15" s="5">
@@ -2334,35 +2364,35 @@
         <v>-795.45666666666682</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Y15" s="5">
@@ -2370,7 +2400,7 @@
         <v>-795.45666666666682</v>
       </c>
       <c r="Z15" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA15" s="5"/>
@@ -2393,99 +2423,99 @@
         <v>-125</v>
       </c>
       <c r="C16" s="8">
-        <f t="shared" ref="C16:Z16" si="6">C17+SUM(C20:C22)</f>
+        <f t="shared" ref="C16:Z16" si="7">C17+SUM(C20:C22)</f>
         <v>-125</v>
       </c>
       <c r="D16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="E16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="F16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="G16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="H16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="I16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-291.66666666666669</v>
       </c>
       <c r="J16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="K16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="L16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="M16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-625</v>
       </c>
       <c r="N16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="O16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="P16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-291.66666666666669</v>
       </c>
       <c r="Q16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="R16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="S16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="T16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="U16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="V16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="W16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="X16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-125</v>
       </c>
       <c r="Y16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-791.66666666666663</v>
       </c>
       <c r="Z16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AA16" s="5"/>
@@ -2508,99 +2538,99 @@
         <v>-41.666666666666664</v>
       </c>
       <c r="C17" s="8">
-        <f t="shared" ref="C17:Z17" si="7">SUM(C18:C19)</f>
+        <f t="shared" ref="C17:Z17" si="8">SUM(C18:C19)</f>
         <v>-41.666666666666664</v>
       </c>
       <c r="D17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="E17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="G17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="H17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="I17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="J17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="K17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="L17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="M17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="N17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="O17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="P17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="Q17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="R17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="S17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="T17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="U17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="V17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="W17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="X17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="Y17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-41.666666666666664</v>
       </c>
       <c r="Z17" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA17" s="5"/>
@@ -2623,95 +2653,95 @@
         <v>-31.25</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" ref="C18:Y18" si="8">-750/24</f>
+        <f t="shared" ref="C18:Y18" si="9">-750/24</f>
         <v>-31.25</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="G18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="I18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="K18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="L18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="M18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="N18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="O18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="P18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="Q18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="R18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="S18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="T18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="U18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="V18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="W18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="X18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="Y18" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>-31.25</v>
       </c>
       <c r="Z18" s="5">
@@ -2737,95 +2767,95 @@
         <v>-10.416666666666666</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" ref="C19:Y19" si="9">-250/24</f>
+        <f t="shared" ref="C19:Y19" si="10">-250/24</f>
         <v>-10.416666666666666</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="G19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="I19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="K19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="L19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="M19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="N19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="O19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="P19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="Q19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="R19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="S19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="T19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="U19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="V19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="W19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="X19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="Y19" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-10.416666666666666</v>
       </c>
       <c r="Z19" s="5">
@@ -3034,95 +3064,95 @@
         <v>-83.333333333333329</v>
       </c>
       <c r="C22" s="8">
-        <f t="shared" ref="C22:Y22" si="10">-2000/24</f>
+        <f t="shared" ref="C22:Y22" si="11">-2000/24</f>
         <v>-83.333333333333329</v>
       </c>
       <c r="D22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="E22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="F22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="G22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="H22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="I22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="J22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="K22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="L22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="M22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="N22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="O22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="P22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="Q22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="R22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="S22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="T22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="U22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="V22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="W22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="X22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="Y22" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-83.333333333333329</v>
       </c>
       <c r="Z22" s="8">
@@ -3144,104 +3174,104 @@
         <v>30</v>
       </c>
       <c r="B23" s="8">
-        <f>B3+B6+B16</f>
-        <v>-87921.21166666667</v>
+        <f>B3+B6+B16+B2</f>
+        <v>-187921.21166666667</v>
       </c>
       <c r="C23" s="8">
-        <f t="shared" ref="C23:Y23" si="11">C3+C6+C16</f>
-        <v>-67268.044999999998</v>
+        <f t="shared" ref="C23:Y23" si="12">C3+C6+C16</f>
+        <v>-67269.544999999998</v>
       </c>
       <c r="D23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67266.544999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="E23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67265.044999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="F23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67263.544999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="G23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67262.044999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="H23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67260.544999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="I23" s="8">
-        <f t="shared" si="11"/>
-        <v>-69812.081666666665</v>
+        <f t="shared" si="12"/>
+        <v>-69822.581666666665</v>
       </c>
       <c r="J23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67257.544999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="K23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67256.044999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="L23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67254.544999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="M23" s="8">
-        <f t="shared" si="11"/>
-        <v>-70698.044999999998</v>
+        <f t="shared" si="12"/>
+        <v>-70714.544999999998</v>
       </c>
       <c r="N23" s="8">
         <f>N3+N6+N16+N2</f>
-        <v>1432748.4550000001</v>
+        <v>1432730.4550000001</v>
       </c>
       <c r="O23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67250.044999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="P23" s="8">
-        <f t="shared" si="11"/>
-        <v>-69801.581666666665</v>
+        <f t="shared" si="12"/>
+        <v>-69822.581666666665</v>
       </c>
       <c r="Q23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67247.044999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="R23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67245.544999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="S23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67244.044999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="T23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67242.544999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="U23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67241.044999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="V23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67239.544999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="W23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67238.044999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="X23" s="8">
-        <f t="shared" si="11"/>
-        <v>-67236.544999999998</v>
+        <f t="shared" si="12"/>
+        <v>-67269.544999999998</v>
       </c>
       <c r="Y23" s="8">
-        <f t="shared" si="11"/>
-        <v>-70288.081666666665</v>
+        <f t="shared" si="12"/>
+        <v>-70322.581666666665</v>
       </c>
       <c r="Z23" s="8">
         <f>Z2</f>
-        <v>1500000</v>
+        <v>1687159.6400000001</v>
       </c>
       <c r="AA23" s="5"/>
       <c r="AB23" s="5"/>
@@ -3262,10 +3292,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3285,103 +3315,103 @@
       </c>
       <c r="B1" s="8">
         <f>'Flujo de Caja'!B23</f>
-        <v>-87921.21166666667</v>
+        <v>-187921.21166666667</v>
       </c>
       <c r="C1" s="8">
         <f>'Flujo de Caja'!C23</f>
-        <v>-67268.044999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="D1" s="8">
         <f>'Flujo de Caja'!D23</f>
-        <v>-67266.544999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="E1" s="8">
         <f>'Flujo de Caja'!E23</f>
-        <v>-67265.044999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="F1" s="8">
         <f>'Flujo de Caja'!F23</f>
-        <v>-67263.544999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="G1" s="8">
         <f>'Flujo de Caja'!G23</f>
-        <v>-67262.044999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="H1" s="8">
         <f>'Flujo de Caja'!H23</f>
-        <v>-67260.544999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="I1" s="8">
         <f>'Flujo de Caja'!I23</f>
-        <v>-69812.081666666665</v>
+        <v>-69822.581666666665</v>
       </c>
       <c r="J1" s="8">
         <f>'Flujo de Caja'!J23</f>
-        <v>-67257.544999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="K1" s="8">
         <f>'Flujo de Caja'!K23</f>
-        <v>-67256.044999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="L1" s="8">
         <f>'Flujo de Caja'!L23</f>
-        <v>-67254.544999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="M1" s="8">
         <f>'Flujo de Caja'!M23</f>
-        <v>-70698.044999999998</v>
+        <v>-70714.544999999998</v>
       </c>
       <c r="N1" s="8">
         <f>'Flujo de Caja'!N23</f>
-        <v>1432748.4550000001</v>
+        <v>1432730.4550000001</v>
       </c>
       <c r="O1" s="8">
         <f>'Flujo de Caja'!O23</f>
-        <v>-67250.044999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="P1" s="8">
         <f>'Flujo de Caja'!P23</f>
-        <v>-69801.581666666665</v>
+        <v>-69822.581666666665</v>
       </c>
       <c r="Q1" s="8">
         <f>'Flujo de Caja'!Q23</f>
-        <v>-67247.044999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="R1" s="8">
         <f>'Flujo de Caja'!R23</f>
-        <v>-67245.544999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="S1" s="8">
         <f>'Flujo de Caja'!S23</f>
-        <v>-67244.044999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="T1" s="8">
         <f>'Flujo de Caja'!T23</f>
-        <v>-67242.544999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="U1" s="8">
         <f>'Flujo de Caja'!U23</f>
-        <v>-67241.044999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="V1" s="8">
         <f>'Flujo de Caja'!V23</f>
-        <v>-67239.544999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="W1" s="8">
         <f>'Flujo de Caja'!W23</f>
-        <v>-67238.044999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="X1" s="8">
         <f>'Flujo de Caja'!X23</f>
-        <v>-67236.544999999998</v>
+        <v>-67269.544999999998</v>
       </c>
       <c r="Y1" s="8">
         <f>'Flujo de Caja'!Y23</f>
-        <v>-70288.081666666665</v>
+        <v>-70322.581666666665</v>
       </c>
       <c r="Z1" s="8">
         <f>'Flujo de Caja'!Z23</f>
-        <v>1500000</v>
+        <v>1687159.6400000001</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -3467,103 +3497,103 @@
       </c>
       <c r="B3" s="5">
         <f>B1</f>
-        <v>-87921.21166666667</v>
+        <v>-187921.21166666667</v>
       </c>
       <c r="C3" s="5">
         <f>B3+C1</f>
-        <v>-155189.25666666665</v>
+        <v>-255190.75666666665</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" ref="D3:Z3" si="0">C3+D1</f>
-        <v>-222455.80166666664</v>
+        <v>-322460.30166666664</v>
       </c>
       <c r="E3" s="5">
         <f t="shared" si="0"/>
-        <v>-289720.84666666662</v>
+        <v>-389729.84666666662</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" si="0"/>
-        <v>-356984.3916666666</v>
+        <v>-456999.3916666666</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="0"/>
-        <v>-424246.43666666659</v>
+        <v>-524268.93666666659</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="0"/>
-        <v>-491506.98166666657</v>
+        <v>-591538.48166666657</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" si="0"/>
-        <v>-561319.06333333324</v>
+        <v>-661361.06333333324</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" si="0"/>
-        <v>-628576.60833333328</v>
+        <v>-728630.60833333328</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" si="0"/>
-        <v>-695832.65333333332</v>
+        <v>-795900.15333333332</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" si="0"/>
-        <v>-763087.19833333336</v>
+        <v>-863169.69833333336</v>
       </c>
       <c r="M3" s="5">
         <f t="shared" si="0"/>
-        <v>-833785.2433333334</v>
+        <v>-933884.2433333334</v>
       </c>
       <c r="N3" s="5">
         <f t="shared" si="0"/>
-        <v>598963.21166666667</v>
+        <v>498846.21166666667</v>
       </c>
       <c r="O3" s="5">
         <f t="shared" si="0"/>
-        <v>531713.16666666663</v>
+        <v>431576.66666666669</v>
       </c>
       <c r="P3" s="5">
         <f t="shared" si="0"/>
-        <v>461911.58499999996</v>
+        <v>361754.08500000002</v>
       </c>
       <c r="Q3" s="5">
         <f t="shared" si="0"/>
-        <v>394664.54</v>
+        <v>294484.54000000004</v>
       </c>
       <c r="R3" s="5">
         <f t="shared" si="0"/>
-        <v>327418.995</v>
+        <v>227214.99500000005</v>
       </c>
       <c r="S3" s="5">
         <f t="shared" si="0"/>
-        <v>260174.95</v>
+        <v>159945.45000000007</v>
       </c>
       <c r="T3" s="5">
         <f t="shared" si="0"/>
-        <v>192932.40500000003</v>
+        <v>92675.905000000072</v>
       </c>
       <c r="U3" s="5">
         <f t="shared" si="0"/>
-        <v>125691.36000000003</v>
+        <v>25406.360000000073</v>
       </c>
       <c r="V3" s="5">
         <f t="shared" si="0"/>
-        <v>58451.815000000031</v>
+        <v>-41863.184999999925</v>
       </c>
       <c r="W3" s="5">
         <f t="shared" si="0"/>
-        <v>-8786.2299999999668</v>
+        <v>-109132.72999999992</v>
       </c>
       <c r="X3" s="5">
         <f t="shared" si="0"/>
-        <v>-76022.774999999965</v>
+        <v>-176402.27499999991</v>
       </c>
       <c r="Y3" s="5">
         <f t="shared" si="0"/>
-        <v>-146310.85666666663</v>
+        <v>-246724.85666666657</v>
       </c>
       <c r="Z3" s="5">
         <f t="shared" si="0"/>
-        <v>1353689.1433333333</v>
+        <v>1440434.7833333337</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -3580,39 +3610,39 @@
       </c>
       <c r="B7" s="5">
         <f>B3</f>
-        <v>-87921.21166666667</v>
+        <v>-187921.21166666667</v>
       </c>
       <c r="E7" s="5">
         <f>E3/(1+B5)</f>
-        <v>-267887.97657574352</v>
+        <v>-360360.46848512866</v>
       </c>
       <c r="H7" s="5">
         <f>H3/(1+B5)^2</f>
-        <v>-420219.92764596752</v>
+        <v>-505743.08654348511</v>
       </c>
       <c r="K7" s="5">
         <f>K3/(1+B5)^3</f>
-        <v>-550079.21304703911</v>
+        <v>-629185.95140991337</v>
       </c>
       <c r="N7" s="5">
         <f>N3/(1+B5)^4</f>
-        <v>437818.44457304658</v>
+        <v>364636.87288127199</v>
       </c>
       <c r="Q7" s="5">
         <f>Q3/(1+B5)^5</f>
-        <v>266744.50927746232</v>
+        <v>199035.19609868986</v>
       </c>
       <c r="T7" s="5">
         <f>T3/(1+B5)^6</f>
-        <v>120571.8807623741</v>
+        <v>57917.218039163075</v>
       </c>
       <c r="W7" s="5">
         <f>W3/(1+B5)^7</f>
-        <v>-5077.1138396961087</v>
+        <v>-63062.234183127504</v>
       </c>
       <c r="Z7" s="5">
         <f>Z3/(1+B5)^8</f>
-        <v>723280.49866417598</v>
+        <v>769628.97539174161</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -3650,15 +3680,95 @@
       </c>
       <c r="B10" s="8">
         <f>SUM(B7:Z7)</f>
-        <v>217229.89050194598</v>
+        <v>-355054.68987745466</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="20">
-        <v>0.12255000000000001</v>
+      <c r="B12" s="21">
+        <v>2.6460000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>100000</v>
+      </c>
+      <c r="E14" s="5">
+        <f>B14*(1+$B$5)</f>
+        <v>108149.99999999999</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5">
+        <f t="shared" ref="F14:Z14" si="1">E14*(1+$B$5)</f>
+        <v>116964.22499999998</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5">
+        <f t="shared" si="1"/>
+        <v>126496.80933749996</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5">
+        <f t="shared" si="1"/>
+        <v>136806.2992985062</v>
+      </c>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5">
+        <f t="shared" si="1"/>
+        <v>147956.01269133444</v>
+      </c>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5">
+        <f t="shared" si="1"/>
+        <v>160014.42772567819</v>
+      </c>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5">
+        <f t="shared" si="1"/>
+        <v>173055.60358532096</v>
+      </c>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5">
+        <f t="shared" si="1"/>
+        <v>187159.63527752459</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="N15">
+        <v>4</v>
+      </c>
+      <c r="Q15">
+        <v>5</v>
+      </c>
+      <c r="T15">
+        <v>6</v>
+      </c>
+      <c r="W15">
+        <v>7</v>
+      </c>
+      <c r="Z15">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>